<commit_message>
Math FLs updated for Grade 7
</commit_message>
<xml_diff>
--- a/PowerSchool Changes.xlsx
+++ b/PowerSchool Changes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawalker\Desktop\PS Configuration 2022-10-28\Customizations - Working files\FLs\Plug-in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0538555-C0B5-4EB2-9BE1-E44776237BDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B8CC05-A199-4046-8C49-654401439155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-135" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{C48B547E-60FC-4B10-AD50-9E1C7BD1A3DB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="304">
   <si>
     <t>PowerSchool</t>
   </si>
@@ -1743,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D39CF3-5255-4B2F-A16B-A7731BE219C0}">
   <dimension ref="A1:M153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F109" sqref="F109"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8"/>
@@ -3125,9 +3125,17 @@
         <v>178</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
-      <c r="A97" t="s">
+    <row r="97" spans="1:12" s="31" customFormat="1">
+      <c r="A97" s="30" t="s">
         <v>179</v>
+      </c>
+      <c r="B97" s="30"/>
+      <c r="C97" s="30"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="30"/>
+      <c r="F97" s="30"/>
+      <c r="G97" s="31" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -3391,9 +3399,17 @@
       <c r="K109" s="15"/>
       <c r="L109" s="15"/>
     </row>
-    <row r="113" spans="1:12">
-      <c r="A113" t="s">
+    <row r="113" spans="1:12" s="31" customFormat="1">
+      <c r="A113" s="30" t="s">
         <v>214</v>
+      </c>
+      <c r="B113" s="30"/>
+      <c r="C113" s="30"/>
+      <c r="D113" s="30"/>
+      <c r="E113" s="30"/>
+      <c r="F113" s="30"/>
+      <c r="G113" s="31" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="115" spans="1:12">
@@ -4115,6 +4131,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="E145:F145"/>
+    <mergeCell ref="H145:I145"/>
+    <mergeCell ref="K145:L145"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="H115:I115"/>
+    <mergeCell ref="K115:L115"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="E130:F130"/>
+    <mergeCell ref="H130:I130"/>
+    <mergeCell ref="K130:L130"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="K81:L81"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="K99:L99"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="E63:F63"/>
     <mergeCell ref="H63:I63"/>
@@ -4131,26 +4167,6 @@
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="H43:I43"/>
     <mergeCell ref="K43:L43"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="K81:L81"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="K99:L99"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="E145:F145"/>
-    <mergeCell ref="H145:I145"/>
-    <mergeCell ref="K145:L145"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="E115:F115"/>
-    <mergeCell ref="H115:I115"/>
-    <mergeCell ref="K115:L115"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="E130:F130"/>
-    <mergeCell ref="H130:I130"/>
-    <mergeCell ref="K130:L130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed math numbering changes - ready for testing.
</commit_message>
<xml_diff>
--- a/PowerSchool Changes.xlsx
+++ b/PowerSchool Changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawalker\Desktop\PS Configuration 2022-10-28\Customizations - Working files\FLs\Plug-in\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukewalker/Sync/DELL Projects/FLs/pei_foundational_learnings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B8CC05-A199-4046-8C49-654401439155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB0D13D-5CD9-C549-8078-E21698EE6FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{C48B547E-60FC-4B10-AD50-9E1C7BD1A3DB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{C48B547E-60FC-4B10-AD50-9E1C7BD1A3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="304">
   <si>
     <t>PowerSchool</t>
   </si>
@@ -1162,7 +1162,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1743,23 +1743,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D39CF3-5255-4B2F-A16B-A7731BE219C0}">
   <dimension ref="A1:M153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="G114" sqref="G114"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="G143" sqref="G143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.296875" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.69921875" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="31" customFormat="1">
+    <row r="7" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>7</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="36" t="s">
         <v>9</v>
       </c>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="I9" s="35"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="I13" s="37"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
         <v>29</v>
       </c>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="I14" s="37"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
         <v>36</v>
       </c>
@@ -1924,7 +1924,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
         <v>37</v>
       </c>
@@ -1933,7 +1933,7 @@
       </c>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
         <v>38</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
         <v>39</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
         <v>41</v>
       </c>
@@ -1957,11 +1957,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B21" s="4"/>
       <c r="C21" s="13"/>
     </row>
-    <row r="24" spans="1:12" s="31" customFormat="1">
+    <row r="24" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
         <v>43</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B26" s="36" t="s">
         <v>9</v>
       </c>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="L26" s="36"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
         <v>12</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
         <v>45</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
         <v>50</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
         <v>55</v>
       </c>
@@ -2107,7 +2107,7 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
         <v>58</v>
       </c>
@@ -2132,7 +2132,7 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
         <v>63</v>
       </c>
@@ -2153,7 +2153,7 @@
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
         <v>65</v>
       </c>
@@ -2174,7 +2174,7 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
         <v>68</v>
       </c>
@@ -2195,7 +2195,7 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
         <v>70</v>
       </c>
@@ -2216,7 +2216,7 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>72</v>
       </c>
@@ -2238,7 +2238,7 @@
       <c r="L36" s="15"/>
       <c r="M36" s="16"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
         <v>75</v>
       </c>
@@ -2255,7 +2255,7 @@
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
     </row>
-    <row r="41" spans="1:13" s="31" customFormat="1">
+    <row r="41" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="30" t="s">
         <v>77</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B43" s="36" t="s">
         <v>9</v>
       </c>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="L43" s="36"/>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B44" s="5" t="s">
         <v>12</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B45" s="7" t="s">
         <v>78</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B46" s="7" t="s">
         <v>83</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B47" s="7" t="s">
         <v>89</v>
       </c>
@@ -2401,7 +2401,7 @@
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B48" s="7" t="s">
         <v>92</v>
       </c>
@@ -2422,7 +2422,7 @@
       <c r="K48" s="15"/>
       <c r="L48" s="15"/>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B49" s="7" t="s">
         <v>94</v>
       </c>
@@ -2441,7 +2441,7 @@
       <c r="K49" s="15"/>
       <c r="L49" s="15"/>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B50" s="7" t="s">
         <v>97</v>
       </c>
@@ -2460,7 +2460,7 @@
       <c r="K50" s="15"/>
       <c r="L50" s="15"/>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B51" s="7" t="s">
         <v>99</v>
       </c>
@@ -2479,7 +2479,7 @@
       <c r="K51" s="15"/>
       <c r="L51" s="15"/>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B52" s="7" t="s">
         <v>101</v>
       </c>
@@ -2494,7 +2494,7 @@
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B53" s="17" t="s">
         <v>102</v>
       </c>
@@ -2509,7 +2509,7 @@
       <c r="K53" s="15"/>
       <c r="L53" s="15"/>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B54" s="17" t="s">
         <v>104</v>
       </c>
@@ -2524,7 +2524,7 @@
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B55" s="17" t="s">
         <v>106</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B56" s="17" t="s">
         <v>108</v>
       </c>
@@ -2542,7 +2542,7 @@
       <c r="E56" s="15"/>
       <c r="F56" s="15"/>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B57" s="7" t="s">
         <v>110</v>
       </c>
@@ -2551,7 +2551,7 @@
       </c>
       <c r="H57" s="21"/>
     </row>
-    <row r="61" spans="1:12" s="33" customFormat="1">
+    <row r="61" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="34" t="s">
         <v>111</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B63" s="35" t="s">
         <v>9</v>
       </c>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="L63" s="36"/>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B64" s="5" t="s">
         <v>12</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B65" s="6" t="s">
         <v>112</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B66" s="6" t="s">
         <v>117</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B67" s="6" t="s">
         <v>121</v>
       </c>
@@ -2697,7 +2697,7 @@
       <c r="K67" s="15"/>
       <c r="L67" s="15"/>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B68" s="6" t="s">
         <v>126</v>
       </c>
@@ -2722,7 +2722,7 @@
       <c r="K68" s="15"/>
       <c r="L68" s="15"/>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B69" s="6" t="s">
         <v>129</v>
       </c>
@@ -2747,7 +2747,7 @@
       <c r="K69" s="15"/>
       <c r="L69" s="15"/>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B70" s="6" t="s">
         <v>133</v>
       </c>
@@ -2772,7 +2772,7 @@
       <c r="K70" s="15"/>
       <c r="L70" s="15"/>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B71" s="6" t="s">
         <v>137</v>
       </c>
@@ -2789,7 +2789,7 @@
       <c r="K71" s="15"/>
       <c r="L71" s="15"/>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B72" s="6" t="s">
         <v>139</v>
       </c>
@@ -2804,7 +2804,7 @@
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B73" s="6" t="s">
         <v>141</v>
       </c>
@@ -2819,7 +2819,7 @@
       <c r="K73" s="15"/>
       <c r="L73" s="15"/>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B74" s="6" t="s">
         <v>143</v>
       </c>
@@ -2834,7 +2834,7 @@
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B75" s="6" t="s">
         <v>144</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:12" s="33" customFormat="1">
+    <row r="79" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="34" t="s">
         <v>145</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="81" spans="2:12">
+    <row r="81" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B81" s="35" t="s">
         <v>9</v>
       </c>
@@ -2876,7 +2876,7 @@
       </c>
       <c r="L81" s="36"/>
     </row>
-    <row r="82" spans="2:12">
+    <row r="82" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B82" s="5" t="s">
         <v>146</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="2:12">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B83" s="6" t="s">
         <v>147</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="84" spans="2:12">
+    <row r="84" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B84" s="6" t="s">
         <v>152</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="85" spans="2:12">
+    <row r="85" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B85" s="6" t="s">
         <v>158</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="2:12">
+    <row r="86" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B86" s="6" t="s">
         <v>161</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="2:12">
+    <row r="87" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B87" s="6" t="s">
         <v>164</v>
       </c>
@@ -3030,7 +3030,7 @@
       <c r="K87" s="15"/>
       <c r="L87" s="15"/>
     </row>
-    <row r="88" spans="2:12">
+    <row r="88" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B88" s="6" t="s">
         <v>167</v>
       </c>
@@ -3049,7 +3049,7 @@
       <c r="K88" s="15"/>
       <c r="L88" s="15"/>
     </row>
-    <row r="89" spans="2:12">
+    <row r="89" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B89" s="6" t="s">
         <v>170</v>
       </c>
@@ -3068,7 +3068,7 @@
       <c r="K89" s="15"/>
       <c r="L89" s="15"/>
     </row>
-    <row r="90" spans="2:12">
+    <row r="90" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B90" s="6" t="s">
         <v>173</v>
       </c>
@@ -3087,7 +3087,7 @@
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
     </row>
-    <row r="91" spans="2:12">
+    <row r="91" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B91" s="6" t="s">
         <v>175</v>
       </c>
@@ -3102,7 +3102,7 @@
       <c r="K91" s="15"/>
       <c r="L91" s="15"/>
     </row>
-    <row r="92" spans="2:12">
+    <row r="92" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B92" s="6" t="s">
         <v>177</v>
       </c>
@@ -3117,7 +3117,7 @@
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
     </row>
-    <row r="93" spans="2:12">
+    <row r="93" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B93" s="6" t="s">
         <v>178</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="97" spans="1:12" s="31" customFormat="1">
+    <row r="97" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="30" t="s">
         <v>179</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B99" s="35" t="s">
         <v>9</v>
       </c>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="L99" s="36"/>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B100" s="5" t="s">
         <v>146</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B101" s="6" t="s">
         <v>180</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="102" spans="1:12">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B102" s="6" t="s">
         <v>186</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="103" spans="1:12">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B103" s="11" t="s">
         <v>191</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="104" spans="1:12">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B104" s="11" t="s">
         <v>197</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B105" s="6" t="s">
         <v>202</v>
       </c>
@@ -3323,7 +3323,7 @@
       <c r="K105" s="15"/>
       <c r="L105" s="15"/>
     </row>
-    <row r="106" spans="1:12">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B106" s="6" t="s">
         <v>204</v>
       </c>
@@ -3342,7 +3342,7 @@
       <c r="K106" s="15"/>
       <c r="L106" s="15"/>
     </row>
-    <row r="107" spans="1:12">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B107" s="11" t="s">
         <v>206</v>
       </c>
@@ -3361,7 +3361,7 @@
       <c r="K107" s="15"/>
       <c r="L107" s="15"/>
     </row>
-    <row r="108" spans="1:12">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B108" s="11" t="s">
         <v>209</v>
       </c>
@@ -3380,7 +3380,7 @@
       <c r="K108" s="4"/>
       <c r="L108" s="4"/>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B109" s="6" t="s">
         <v>212</v>
       </c>
@@ -3399,7 +3399,7 @@
       <c r="K109" s="15"/>
       <c r="L109" s="15"/>
     </row>
-    <row r="113" spans="1:12" s="31" customFormat="1">
+    <row r="113" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="30" t="s">
         <v>214</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B115" s="35" t="s">
         <v>9</v>
       </c>
@@ -3433,7 +3433,7 @@
       </c>
       <c r="L115" s="36"/>
     </row>
-    <row r="116" spans="1:12">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B116" s="5" t="s">
         <v>146</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B117" s="6" t="s">
         <v>215</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="118" spans="1:12">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B118" s="6" t="s">
         <v>220</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B119" s="6" t="s">
         <v>225</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B120" s="6" t="s">
         <v>229</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B121" s="6" t="s">
         <v>234</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="122" spans="1:12">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B122" s="11" t="s">
         <v>238</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B123" s="23" t="s">
         <v>242</v>
       </c>
@@ -3651,7 +3651,7 @@
       <c r="K123" s="15"/>
       <c r="L123" s="15"/>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B124" s="11" t="s">
         <v>246</v>
       </c>
@@ -3664,12 +3664,20 @@
       <c r="K124" s="4"/>
       <c r="L124" s="4"/>
     </row>
-    <row r="128" spans="1:12">
-      <c r="A128" t="s">
+    <row r="128" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="30" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="130" spans="1:12">
+      <c r="B128" s="30"/>
+      <c r="C128" s="30"/>
+      <c r="D128" s="30"/>
+      <c r="E128" s="30"/>
+      <c r="F128" s="30"/>
+      <c r="G128" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B130" s="35" t="s">
         <v>9</v>
       </c>
@@ -3690,7 +3698,7 @@
       </c>
       <c r="L130" s="36"/>
     </row>
-    <row r="131" spans="1:12">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B131" s="5" t="s">
         <v>146</v>
       </c>
@@ -3719,7 +3727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="132" spans="1:12">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B132" s="6" t="s">
         <v>249</v>
       </c>
@@ -3748,7 +3756,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="133" spans="1:12">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B133" s="6" t="s">
         <v>254</v>
       </c>
@@ -3777,7 +3785,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="134" spans="1:12">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B134" s="6" t="s">
         <v>259</v>
       </c>
@@ -3798,7 +3806,7 @@
       <c r="K134" s="4"/>
       <c r="L134" s="26"/>
     </row>
-    <row r="135" spans="1:12">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B135" s="6" t="s">
         <v>261</v>
       </c>
@@ -3819,7 +3827,7 @@
       <c r="K135" s="4"/>
       <c r="L135" s="13"/>
     </row>
-    <row r="136" spans="1:12">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B136" s="11" t="s">
         <v>263</v>
       </c>
@@ -3840,7 +3848,7 @@
       <c r="K136" s="4"/>
       <c r="L136" s="13"/>
     </row>
-    <row r="137" spans="1:12">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B137" s="27" t="s">
         <v>234</v>
       </c>
@@ -3861,7 +3869,7 @@
       <c r="K137" s="4"/>
       <c r="L137" s="26"/>
     </row>
-    <row r="138" spans="1:12">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B138" s="11" t="s">
         <v>268</v>
       </c>
@@ -3876,7 +3884,7 @@
       <c r="K138" s="15"/>
       <c r="L138" s="15"/>
     </row>
-    <row r="139" spans="1:12">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B139" s="6" t="s">
         <v>242</v>
       </c>
@@ -3889,12 +3897,20 @@
       <c r="K139" s="4"/>
       <c r="L139" s="4"/>
     </row>
-    <row r="143" spans="1:12">
-      <c r="A143" t="s">
+    <row r="143" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="30" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="145" spans="2:12">
+      <c r="B143" s="30"/>
+      <c r="C143" s="30"/>
+      <c r="D143" s="30"/>
+      <c r="E143" s="30"/>
+      <c r="F143" s="30"/>
+      <c r="G143" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B145" s="35" t="s">
         <v>9</v>
       </c>
@@ -3915,7 +3931,7 @@
       </c>
       <c r="L145" s="36"/>
     </row>
-    <row r="146" spans="2:12">
+    <row r="146" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B146" s="25" t="s">
         <v>146</v>
       </c>
@@ -3944,7 +3960,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="2:12">
+    <row r="147" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B147" s="6" t="s">
         <v>271</v>
       </c>
@@ -3973,7 +3989,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="148" spans="2:12">
+    <row r="148" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B148" s="6" t="s">
         <v>276</v>
       </c>
@@ -4002,7 +4018,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="149" spans="2:12">
+    <row r="149" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B149" s="6" t="s">
         <v>281</v>
       </c>
@@ -4031,7 +4047,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="150" spans="2:12">
+    <row r="150" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B150" s="6" t="s">
         <v>287</v>
       </c>
@@ -4060,7 +4076,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="151" spans="2:12">
+    <row r="151" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B151" s="29" t="s">
         <v>249</v>
       </c>
@@ -4085,7 +4101,7 @@
       <c r="K151" s="4"/>
       <c r="L151" s="13"/>
     </row>
-    <row r="152" spans="2:12">
+    <row r="152" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B152" s="6" t="s">
         <v>292</v>
       </c>
@@ -4110,7 +4126,7 @@
       <c r="K152" s="4"/>
       <c r="L152" s="26"/>
     </row>
-    <row r="153" spans="2:12">
+    <row r="153" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B153" s="6" t="s">
         <v>295</v>
       </c>
@@ -4131,26 +4147,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="E145:F145"/>
-    <mergeCell ref="H145:I145"/>
-    <mergeCell ref="K145:L145"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="E115:F115"/>
-    <mergeCell ref="H115:I115"/>
-    <mergeCell ref="K115:L115"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="E130:F130"/>
-    <mergeCell ref="H130:I130"/>
-    <mergeCell ref="K130:L130"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="K81:L81"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="K99:L99"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="E63:F63"/>
     <mergeCell ref="H63:I63"/>
@@ -4167,6 +4163,26 @@
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="H43:I43"/>
     <mergeCell ref="K43:L43"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="K81:L81"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="K99:L99"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="E145:F145"/>
+    <mergeCell ref="H145:I145"/>
+    <mergeCell ref="K145:L145"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="H115:I115"/>
+    <mergeCell ref="K115:L115"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="E130:F130"/>
+    <mergeCell ref="H130:I130"/>
+    <mergeCell ref="K130:L130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Additional edits to Math FLs to match new values.
</commit_message>
<xml_diff>
--- a/PowerSchool Changes.xlsx
+++ b/PowerSchool Changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukewalker/Sync/DELL Projects/FLs/pei_foundational_learnings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawalker\Desktop\PS Configuration 2022-10-28\Customizations - Working files\FLs\Plug-in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB0D13D-5CD9-C549-8078-E21698EE6FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25FF49D-5DF6-4536-8321-498057773C4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{C48B547E-60FC-4B10-AD50-9E1C7BD1A3DB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{C48B547E-60FC-4B10-AD50-9E1C7BD1A3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     </r>
   </si>
   <si>
-    <t>Changes made but not tested.</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -1157,12 +1154,15 @@
   <si>
     <t>No changes to Grade 5.</t>
   </si>
+  <si>
+    <t>Changes made and deployed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1213,7 +1213,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1235,18 +1235,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1312,7 +1300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1395,9 +1383,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1407,6 +1392,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1743,23 +1729,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D39CF3-5255-4B2F-A16B-A7731BE219C0}">
   <dimension ref="A1:M153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G143" sqref="G143"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.296875" customWidth="1"/>
     <col min="7" max="7" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.69921875" customWidth="1"/>
+    <col min="11" max="12" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1767,7 +1754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1775,7 +1762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1783,467 +1770,468 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+    <row r="6" spans="1:9" ht="13.2" customHeight="1"/>
+    <row r="7" spans="1:9" s="30" customFormat="1">
+      <c r="A7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="31" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9" s="33" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="36" t="s">
+      <c r="C9" s="33"/>
+      <c r="E9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="E9" s="35" t="s">
+      <c r="F9" s="32"/>
+      <c r="H9" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="35"/>
-      <c r="H9" s="35" t="s">
+      <c r="I9" s="32"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="35"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="E10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="6" t="s">
+      <c r="I11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="6" t="s">
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="7" t="s">
+      <c r="I12" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="37" t="s">
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="H13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="I13" s="34"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="37"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="F14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="I14" s="34"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="37"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="6" t="s">
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="C16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="B17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="B18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="6" t="s">
+    </row>
+    <row r="19" spans="1:12">
+      <c r="B19" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="12" t="s">
+    </row>
+    <row r="20" spans="1:12">
+      <c r="B20" s="11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="11" t="s">
+      <c r="C20" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:12">
       <c r="B21" s="4"/>
       <c r="C21" s="13"/>
     </row>
-    <row r="24" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="30" t="s">
+    <row r="24" spans="1:12" s="30" customFormat="1">
+      <c r="A24" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="B26" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="33"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="32"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="32"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="35"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="35" t="s">
+      <c r="L26" s="33"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="B27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I26" s="35"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="L26" s="36"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:12">
       <c r="B28" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="B29" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="L28" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>52</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="B30" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="L29" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B30" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="B31" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="B32" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="B33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="B34" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="B35" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="B36" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>73</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
       <c r="M36" s="16"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="B37" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -2255,236 +2243,236 @@
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
     </row>
-    <row r="41" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="31" t="s">
+    <row r="41" spans="1:13" s="30" customFormat="1">
+      <c r="A41" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="B43" s="33" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B43" s="36" t="s">
+      <c r="C43" s="33"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="36"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="35" t="s">
+      <c r="F43" s="32"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="F43" s="35"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="35" t="s">
+      <c r="I43" s="32"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L43" s="33"/>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="B44" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I43" s="35"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="L43" s="36"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B44" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I44" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L44" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L44" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:13">
       <c r="B45" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="B46" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="L45" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B46" s="7" t="s">
+      <c r="C46" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F46" s="18" t="s">
         <v>85</v>
-      </c>
-      <c r="F46" s="18" t="s">
-        <v>86</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="L46" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="B47" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="L46" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B47" s="7" t="s">
-        <v>89</v>
-      </c>
       <c r="C47" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13">
       <c r="B48" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="15"/>
       <c r="F48" s="15"/>
       <c r="G48" s="4"/>
       <c r="H48" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="15"/>
       <c r="L48" s="15"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12">
       <c r="B49" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I49" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="I49" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="15"/>
       <c r="L49" s="15"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12">
       <c r="B50" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D50" s="4"/>
       <c r="G50" s="4"/>
       <c r="H50" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="15"/>
       <c r="L50" s="15"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12">
       <c r="B51" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I51" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="15"/>
       <c r="L51" s="15"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12">
       <c r="B52" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D52" s="4"/>
       <c r="G52" s="4"/>
@@ -2494,12 +2482,12 @@
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12">
       <c r="B53" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="18" t="s">
         <v>102</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>103</v>
       </c>
       <c r="D53" s="4"/>
       <c r="G53" s="4"/>
@@ -2509,12 +2497,12 @@
       <c r="K53" s="15"/>
       <c r="L53" s="15"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12">
       <c r="B54" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="18" t="s">
         <v>104</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>105</v>
       </c>
       <c r="D54" s="4"/>
       <c r="G54" s="4"/>
@@ -2524,260 +2512,260 @@
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12">
       <c r="B55" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="18" t="s">
+    </row>
+    <row r="56" spans="1:12">
+      <c r="B56" s="17" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B56" s="17" t="s">
+      <c r="C56" s="18" t="s">
         <v>108</v>
-      </c>
-      <c r="C56" s="18" t="s">
-        <v>109</v>
       </c>
       <c r="E56" s="15"/>
       <c r="F56" s="15"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12">
       <c r="B57" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="H57" s="21"/>
+    </row>
+    <row r="61" spans="1:12" s="30" customFormat="1">
+      <c r="A61" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="C57" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="H57" s="21"/>
-    </row>
-    <row r="61" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="B61" s="34"/>
-      <c r="C61" s="34"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="33" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B63" s="35" t="s">
+      <c r="B61" s="31"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="31"/>
+      <c r="G61" s="30" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="B63" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="32"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C63" s="35"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="35" t="s">
+      <c r="F63" s="32"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="F63" s="35"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="35" t="s">
+      <c r="I63" s="32"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L63" s="33"/>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="B64" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I63" s="35"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="L63" s="36"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B64" s="5" t="s">
+      <c r="C64" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I64" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="I64" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L64" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L64" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:12">
       <c r="B65" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C65" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>113</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G65" s="4"/>
       <c r="H65" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="L65" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="B66" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="L65" s="6" t="s">
+      <c r="C66" s="6" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B66" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>117</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G66" s="4"/>
       <c r="H66" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J66" s="4"/>
       <c r="K66" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="L66" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="B67" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="L66" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B67" s="6" t="s">
+      <c r="C67" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I67" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I67" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J67" s="4"/>
       <c r="K67" s="15"/>
       <c r="L67" s="15"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12">
       <c r="B68" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F68" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G68" s="4"/>
       <c r="H68" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J68" s="4"/>
       <c r="K68" s="15"/>
       <c r="L68" s="15"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12">
       <c r="B69" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C69" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>130</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G69" s="4"/>
       <c r="H69" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I69" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J69" s="4"/>
       <c r="K69" s="15"/>
       <c r="L69" s="15"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12">
       <c r="B70" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>134</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G70" s="4"/>
       <c r="H70" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I70" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J70" s="4"/>
       <c r="K70" s="15"/>
       <c r="L70" s="15"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12">
       <c r="B71" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>138</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -2789,12 +2777,12 @@
       <c r="K71" s="15"/>
       <c r="L71" s="15"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12">
       <c r="B72" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C72" s="6" t="s">
         <v>139</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>140</v>
       </c>
       <c r="D72" s="4"/>
       <c r="G72" s="4"/>
@@ -2804,12 +2792,12 @@
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12">
       <c r="B73" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C73" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>142</v>
       </c>
       <c r="D73" s="4"/>
       <c r="G73" s="4"/>
@@ -2819,12 +2807,12 @@
       <c r="K73" s="15"/>
       <c r="L73" s="15"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12">
       <c r="B74" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D74" s="4"/>
       <c r="G74" s="4"/>
@@ -2834,265 +2822,265 @@
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12">
       <c r="B75" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" s="30" customFormat="1">
+      <c r="A79" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="C75" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="34" t="s">
+      <c r="B79" s="31"/>
+      <c r="C79" s="31"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="31"/>
+      <c r="F79" s="31"/>
+      <c r="G79" s="30" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12">
+      <c r="B81" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" s="32"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="32"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="I81" s="32"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L81" s="33"/>
+    </row>
+    <row r="82" spans="2:12">
+      <c r="B82" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B79" s="34"/>
-      <c r="C79" s="34"/>
-      <c r="D79" s="34"/>
-      <c r="E79" s="34"/>
-      <c r="F79" s="34"/>
-      <c r="G79" s="33" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B81" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="C81" s="35"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F81" s="35"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="I81" s="35"/>
-      <c r="J81" s="4"/>
-      <c r="K81" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="L81" s="36"/>
-    </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B82" s="5" t="s">
-        <v>146</v>
-      </c>
       <c r="C82" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="G82" s="4"/>
       <c r="H82" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I82" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="I82" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="J82" s="4"/>
       <c r="K82" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L82" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L82" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="2:12">
       <c r="B83" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G83" s="4"/>
       <c r="H83" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="I83" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="I83" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="J83" s="4"/>
       <c r="K83" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="L83" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12">
+      <c r="B84" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="L83" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B84" s="6" t="s">
+      <c r="C84" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F84" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="G84" s="4"/>
       <c r="H84" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I84" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J84" s="4"/>
       <c r="K84" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="L84" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12">
+      <c r="B85" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="L84" s="6" t="s">
+      <c r="C85" s="6" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B85" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>158</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
       <c r="H85" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I85" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J85" s="4"/>
       <c r="K85" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="L85" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12">
+      <c r="B86" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="L85" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B86" s="6" t="s">
-        <v>161</v>
-      </c>
       <c r="C86" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D86" s="4"/>
       <c r="G86" s="4"/>
       <c r="H86" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J86" s="4"/>
       <c r="K86" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="L86" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12">
+      <c r="B87" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="L86" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B87" s="6" t="s">
+      <c r="C87" s="6" t="s">
         <v>164</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>165</v>
       </c>
       <c r="D87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J87" s="4"/>
       <c r="K87" s="15"/>
       <c r="L87" s="15"/>
     </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:12">
       <c r="B88" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C88" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>168</v>
       </c>
       <c r="D88" s="4"/>
       <c r="G88" s="4"/>
       <c r="H88" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I88" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J88" s="4"/>
       <c r="K88" s="15"/>
       <c r="L88" s="15"/>
     </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:12">
       <c r="B89" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C89" s="6" t="s">
         <v>170</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>171</v>
       </c>
       <c r="D89" s="4"/>
       <c r="G89" s="4"/>
       <c r="H89" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J89" s="4"/>
       <c r="K89" s="15"/>
       <c r="L89" s="15"/>
     </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:12">
       <c r="B90" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D90" s="4"/>
       <c r="G90" s="4"/>
       <c r="H90" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I90" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J90" s="4"/>
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
     </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:12">
       <c r="B91" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="D91" s="4"/>
       <c r="G91" s="4"/>
@@ -3102,12 +3090,12 @@
       <c r="K91" s="15"/>
       <c r="L91" s="15"/>
     </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:12">
       <c r="B92" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D92" s="4"/>
       <c r="G92" s="4"/>
@@ -3117,546 +3105,546 @@
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
     </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:12">
       <c r="B93" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" s="30" customFormat="1">
+      <c r="A97" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="C93" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="B97" s="30"/>
-      <c r="C97" s="30"/>
-      <c r="D97" s="30"/>
-      <c r="E97" s="30"/>
-      <c r="F97" s="30"/>
-      <c r="G97" s="31" t="s">
+      <c r="B97" s="31"/>
+      <c r="C97" s="31"/>
+      <c r="D97" s="31"/>
+      <c r="E97" s="31"/>
+      <c r="F97" s="31"/>
+      <c r="G97" s="30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
+      <c r="B99" s="32" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B99" s="35" t="s">
+      <c r="C99" s="32"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C99" s="35"/>
-      <c r="D99" s="4"/>
-      <c r="E99" s="35" t="s">
+      <c r="F99" s="32"/>
+      <c r="G99" s="4"/>
+      <c r="H99" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="F99" s="35"/>
-      <c r="G99" s="4"/>
-      <c r="H99" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="I99" s="35"/>
+      <c r="I99" s="32"/>
       <c r="J99" s="4"/>
-      <c r="K99" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="L99" s="36"/>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K99" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L99" s="33"/>
+    </row>
+    <row r="100" spans="1:12">
       <c r="B100" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I100" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J100" s="4"/>
       <c r="K100" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L100" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="B101" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G101" s="4"/>
       <c r="H101" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="I101" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="I101" s="6" t="s">
-        <v>183</v>
       </c>
       <c r="J101" s="4"/>
       <c r="K101" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="L101" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="L101" s="6" t="s">
+    </row>
+    <row r="102" spans="1:12">
+      <c r="B102" s="6" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B102" s="6" t="s">
-        <v>186</v>
-      </c>
       <c r="C102" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F102" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="F102" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="G102" s="4"/>
       <c r="H102" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I102" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J102" s="4"/>
       <c r="K102" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="L102" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
+      <c r="B103" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="L102" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B103" s="11" t="s">
+      <c r="C103" s="12" t="s">
         <v>191</v>
-      </c>
-      <c r="C103" s="12" t="s">
-        <v>192</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="I103" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="I103" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="J103" s="4"/>
       <c r="K103" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="L103" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
+      <c r="B104" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="L103" s="9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B104" s="11" t="s">
+      <c r="C104" s="12" t="s">
         <v>197</v>
-      </c>
-      <c r="C104" s="12" t="s">
-        <v>198</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I104" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J104" s="4"/>
       <c r="K104" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L104" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
+      <c r="B105" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="L104" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B105" s="6" t="s">
-        <v>202</v>
-      </c>
       <c r="C105" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D105" s="4"/>
       <c r="G105" s="4"/>
       <c r="H105" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I105" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J105" s="4"/>
       <c r="K105" s="15"/>
       <c r="L105" s="15"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12">
       <c r="B106" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D106" s="4"/>
       <c r="G106" s="4"/>
       <c r="H106" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I106" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J106" s="4"/>
       <c r="K106" s="15"/>
       <c r="L106" s="15"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12">
       <c r="B107" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="C107" s="12" t="s">
         <v>206</v>
-      </c>
-      <c r="C107" s="12" t="s">
-        <v>207</v>
       </c>
       <c r="D107" s="4"/>
       <c r="G107" s="4"/>
       <c r="H107" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I107" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J107" s="4"/>
       <c r="K107" s="15"/>
       <c r="L107" s="15"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12">
       <c r="B108" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C108" s="12" t="s">
         <v>209</v>
-      </c>
-      <c r="C108" s="12" t="s">
-        <v>210</v>
       </c>
       <c r="D108" s="4"/>
       <c r="G108" s="4"/>
       <c r="H108" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I108" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J108" s="4"/>
       <c r="K108" s="4"/>
       <c r="L108" s="4"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12">
       <c r="B109" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D109" s="4"/>
       <c r="G109" s="4"/>
       <c r="H109" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I109" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J109" s="15"/>
       <c r="K109" s="15"/>
       <c r="L109" s="15"/>
     </row>
-    <row r="113" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="30" t="s">
-        <v>214</v>
-      </c>
-      <c r="B113" s="30"/>
-      <c r="C113" s="30"/>
-      <c r="D113" s="30"/>
-      <c r="E113" s="30"/>
-      <c r="F113" s="30"/>
-      <c r="G113" s="31" t="s">
+    <row r="113" spans="1:12" s="30" customFormat="1">
+      <c r="A113" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="B113" s="31"/>
+      <c r="C113" s="31"/>
+      <c r="D113" s="31"/>
+      <c r="E113" s="31"/>
+      <c r="F113" s="31"/>
+      <c r="G113" s="30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
+      <c r="B115" s="32" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B115" s="35" t="s">
+      <c r="C115" s="32"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C115" s="35"/>
-      <c r="D115" s="4"/>
-      <c r="E115" s="35" t="s">
+      <c r="F115" s="32"/>
+      <c r="G115" s="4"/>
+      <c r="H115" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="F115" s="35"/>
-      <c r="G115" s="4"/>
-      <c r="H115" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="I115" s="35"/>
+      <c r="I115" s="32"/>
       <c r="J115" s="4"/>
-      <c r="K115" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="L115" s="36"/>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K115" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L115" s="33"/>
+    </row>
+    <row r="116" spans="1:12">
       <c r="B116" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G116" s="4"/>
       <c r="H116" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I116" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J116" s="4"/>
       <c r="K116" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L116" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
       <c r="B117" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G117" s="4"/>
       <c r="H117" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="I117" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="I117" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="J117" s="4"/>
       <c r="K117" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="L117" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
+      <c r="B118" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="L117" s="6" t="s">
+      <c r="C118" s="6" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B118" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="C118" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G118" s="4"/>
       <c r="H118" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="I118" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="I118" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="J118" s="4"/>
       <c r="K118" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="L118" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
+      <c r="B119" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="L118" s="6" t="s">
+      <c r="C119" s="6" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B119" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>225</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F119" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G119" s="4"/>
       <c r="H119" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I119" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J119" s="4"/>
       <c r="K119" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="L119" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="B120" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="L119" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B120" s="6" t="s">
-        <v>229</v>
-      </c>
       <c r="C120" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G120" s="4"/>
       <c r="H120" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I120" s="12" t="s">
         <v>231</v>
-      </c>
-      <c r="I120" s="12" t="s">
-        <v>232</v>
       </c>
       <c r="J120" s="4"/>
       <c r="K120" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="L120" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
+      <c r="B121" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="L120" s="9" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B121" s="6" t="s">
-        <v>234</v>
-      </c>
       <c r="C121" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G121" s="4"/>
       <c r="H121" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I121" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J121" s="4"/>
       <c r="K121" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="L121" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="B122" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="L121" s="9" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B122" s="11" t="s">
+      <c r="C122" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="C122" s="12" t="s">
-        <v>239</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G122" s="4"/>
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
       <c r="J122" s="4"/>
       <c r="K122" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="L122" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
+      <c r="B123" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="L122" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B123" s="23" t="s">
+      <c r="C123" s="24" t="s">
         <v>242</v>
-      </c>
-      <c r="C123" s="24" t="s">
-        <v>243</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="F123" s="12" t="s">
         <v>244</v>
-      </c>
-      <c r="F123" s="12" t="s">
-        <v>245</v>
       </c>
       <c r="G123" s="4"/>
       <c r="J123" s="4"/>
       <c r="K123" s="15"/>
       <c r="L123" s="15"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12">
       <c r="B124" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="C124" s="12" t="s">
         <v>246</v>
-      </c>
-      <c r="C124" s="12" t="s">
-        <v>247</v>
       </c>
       <c r="D124" s="4"/>
       <c r="G124" s="4"/>
@@ -3664,217 +3652,217 @@
       <c r="K124" s="4"/>
       <c r="L124" s="4"/>
     </row>
-    <row r="128" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="B128" s="30"/>
-      <c r="C128" s="30"/>
-      <c r="D128" s="30"/>
-      <c r="E128" s="30"/>
-      <c r="F128" s="30"/>
-      <c r="G128" s="31" t="s">
+    <row r="128" spans="1:12" s="30" customFormat="1">
+      <c r="A128" s="31" t="s">
+        <v>247</v>
+      </c>
+      <c r="B128" s="31"/>
+      <c r="C128" s="31"/>
+      <c r="D128" s="31"/>
+      <c r="E128" s="31"/>
+      <c r="F128" s="31"/>
+      <c r="G128" s="30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
+      <c r="B130" s="32" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B130" s="35" t="s">
+      <c r="C130" s="32"/>
+      <c r="D130" s="4"/>
+      <c r="E130" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C130" s="35"/>
-      <c r="D130" s="4"/>
-      <c r="E130" s="35" t="s">
+      <c r="F130" s="32"/>
+      <c r="G130" s="4"/>
+      <c r="H130" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="F130" s="35"/>
-      <c r="G130" s="4"/>
-      <c r="H130" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="I130" s="35"/>
+      <c r="I130" s="32"/>
       <c r="J130" s="4"/>
-      <c r="K130" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="L130" s="36"/>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K130" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L130" s="33"/>
+    </row>
+    <row r="131" spans="1:12">
       <c r="B131" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D131" s="4"/>
       <c r="E131" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F131" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G131" s="4"/>
       <c r="H131" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I131" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J131" s="4"/>
       <c r="K131" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L131" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
       <c r="B132" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="F132" s="6" t="s">
         <v>250</v>
-      </c>
-      <c r="F132" s="6" t="s">
-        <v>251</v>
       </c>
       <c r="G132" s="4"/>
       <c r="H132" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I132" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J132" s="4"/>
       <c r="K132" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="L132" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
+      <c r="B133" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="L132" s="6" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B133" s="6" t="s">
-        <v>254</v>
-      </c>
       <c r="C133" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="F133" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="F133" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="G133" s="4"/>
       <c r="H133" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I133" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J133" s="4"/>
       <c r="K133" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L133" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
+      <c r="B134" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="L133" s="6" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B134" s="6" t="s">
-        <v>259</v>
-      </c>
       <c r="C134" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
       <c r="F134" s="13"/>
       <c r="G134" s="4"/>
       <c r="H134" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I134" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J134" s="4"/>
       <c r="K134" s="4"/>
       <c r="L134" s="26"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12">
       <c r="B135" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
       <c r="F135" s="13"/>
       <c r="G135" s="4"/>
       <c r="H135" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I135" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J135" s="4"/>
       <c r="K135" s="4"/>
       <c r="L135" s="13"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12">
       <c r="B136" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="C136" s="12" t="s">
         <v>263</v>
-      </c>
-      <c r="C136" s="12" t="s">
-        <v>264</v>
       </c>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
       <c r="F136" s="13"/>
       <c r="G136" s="4"/>
       <c r="H136" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I136" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J136" s="4"/>
       <c r="K136" s="4"/>
       <c r="L136" s="13"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12">
       <c r="B137" s="27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C137" s="24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
       <c r="F137" s="13"/>
       <c r="G137" s="4"/>
       <c r="H137" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I137" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J137" s="4"/>
       <c r="K137" s="4"/>
       <c r="L137" s="26"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12">
       <c r="B138" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="C138" s="12" t="s">
         <v>268</v>
-      </c>
-      <c r="C138" s="12" t="s">
-        <v>269</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
@@ -3884,12 +3872,12 @@
       <c r="K138" s="15"/>
       <c r="L138" s="15"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12">
       <c r="B139" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D139" s="4"/>
       <c r="G139" s="4"/>
@@ -3897,248 +3885,248 @@
       <c r="K139" s="4"/>
       <c r="L139" s="4"/>
     </row>
-    <row r="143" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="B143" s="30"/>
-      <c r="C143" s="30"/>
-      <c r="D143" s="30"/>
-      <c r="E143" s="30"/>
-      <c r="F143" s="30"/>
-      <c r="G143" s="31" t="s">
+    <row r="143" spans="1:12" s="30" customFormat="1">
+      <c r="A143" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="B143" s="31"/>
+      <c r="C143" s="31"/>
+      <c r="D143" s="31"/>
+      <c r="E143" s="31"/>
+      <c r="F143" s="31"/>
+      <c r="G143" s="30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="145" spans="2:12">
+      <c r="B145" s="32" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="145" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B145" s="35" t="s">
+      <c r="C145" s="32"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C145" s="35"/>
-      <c r="D145" s="4"/>
-      <c r="E145" s="35" t="s">
+      <c r="F145" s="32"/>
+      <c r="G145" s="4"/>
+      <c r="H145" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="F145" s="35"/>
-      <c r="G145" s="4"/>
-      <c r="H145" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="I145" s="35"/>
+      <c r="I145" s="32"/>
       <c r="J145" s="4"/>
-      <c r="K145" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="L145" s="36"/>
-    </row>
-    <row r="146" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="K145" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L145" s="33"/>
+    </row>
+    <row r="146" spans="2:12">
       <c r="B146" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C146" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D146" s="4"/>
       <c r="E146" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F146" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G146" s="4"/>
       <c r="H146" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I146" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J146" s="4"/>
       <c r="K146" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L146" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="147" spans="2:12" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="147" spans="2:12">
       <c r="B147" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C147" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="C147" s="6" t="s">
-        <v>272</v>
       </c>
       <c r="D147" s="4"/>
       <c r="E147" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F147" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G147" s="4"/>
       <c r="H147" s="28" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I147" s="24" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J147" s="4"/>
       <c r="K147" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="L147" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="148" spans="2:12">
+      <c r="B148" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="L147" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="148" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B148" s="6" t="s">
+      <c r="C148" s="6" t="s">
         <v>276</v>
-      </c>
-      <c r="C148" s="6" t="s">
-        <v>277</v>
       </c>
       <c r="D148" s="4"/>
       <c r="E148" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F148" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G148" s="4"/>
       <c r="H148" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I148" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J148" s="4"/>
       <c r="K148" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="L148" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="149" spans="2:12">
+      <c r="B149" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="L148" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="149" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B149" s="6" t="s">
+      <c r="C149" s="6" t="s">
         <v>281</v>
-      </c>
-      <c r="C149" s="6" t="s">
-        <v>282</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="F149" s="12" t="s">
         <v>283</v>
-      </c>
-      <c r="F149" s="12" t="s">
-        <v>284</v>
       </c>
       <c r="G149" s="4"/>
       <c r="H149" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I149" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J149" s="4"/>
       <c r="K149" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="L149" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="150" spans="2:12">
+      <c r="B150" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="L149" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="150" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B150" s="6" t="s">
+      <c r="C150" s="6" t="s">
         <v>287</v>
-      </c>
-      <c r="C150" s="6" t="s">
-        <v>288</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F150" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G150" s="4"/>
       <c r="H150" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I150" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J150" s="4"/>
       <c r="K150" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="L150" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="151" spans="2:12">
+      <c r="B151" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="C151" s="9" t="s">
         <v>291</v>
-      </c>
-      <c r="L150" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="151" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B151" s="29" t="s">
-        <v>249</v>
-      </c>
-      <c r="C151" s="9" t="s">
-        <v>292</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F151" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G151" s="4"/>
       <c r="H151" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I151" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J151" s="4"/>
       <c r="K151" s="4"/>
       <c r="L151" s="13"/>
     </row>
-    <row r="152" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:12">
       <c r="B152" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D152" s="4"/>
       <c r="E152" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F152" s="12" t="s">
         <v>296</v>
-      </c>
-      <c r="F152" s="12" t="s">
-        <v>297</v>
       </c>
       <c r="G152" s="4"/>
       <c r="H152" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I152" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J152" s="4"/>
       <c r="K152" s="4"/>
       <c r="L152" s="26"/>
     </row>
-    <row r="153" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:12">
       <c r="B153" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D153" s="4"/>
       <c r="E153" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="F153" s="12" t="s">
         <v>300</v>
-      </c>
-      <c r="F153" s="12" t="s">
-        <v>301</v>
       </c>
       <c r="G153" s="4"/>
       <c r="J153" s="4"/>
@@ -4147,6 +4135,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="E145:F145"/>
+    <mergeCell ref="H145:I145"/>
+    <mergeCell ref="K145:L145"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="H115:I115"/>
+    <mergeCell ref="K115:L115"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="E130:F130"/>
+    <mergeCell ref="H130:I130"/>
+    <mergeCell ref="K130:L130"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="K81:L81"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="K99:L99"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="E63:F63"/>
     <mergeCell ref="H63:I63"/>
@@ -4163,26 +4171,6 @@
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="H43:I43"/>
     <mergeCell ref="K43:L43"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="K81:L81"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="K99:L99"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="E145:F145"/>
-    <mergeCell ref="H145:I145"/>
-    <mergeCell ref="K145:L145"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="E115:F115"/>
-    <mergeCell ref="H115:I115"/>
-    <mergeCell ref="K115:L115"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="E130:F130"/>
-    <mergeCell ref="H130:I130"/>
-    <mergeCell ref="K130:L130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>